<commit_message>
Fittings finished and tested
</commit_message>
<xml_diff>
--- a/revit-ntr-exporter/NTR_CONFIG.xlsx
+++ b/revit-ntr-exporter/NTR_CONFIG.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Github\Revit-PCF-Exporter\Revit-NTR-Exporter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Revit-PCF-Exporter\Revit-NTR-Exporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="115">
   <si>
     <t>TMONT</t>
   </si>
@@ -316,6 +316,66 @@
   </si>
   <si>
     <t>EN 10253-2</t>
+  </si>
+  <si>
+    <t>EN 10253-2 - Reducer: Conc.</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>EN 10253-2 - Reducer: Ecc.</t>
+  </si>
+  <si>
+    <t>Flange weld collar: PN40</t>
+  </si>
+  <si>
+    <t>Flange weld collar: PN06</t>
+  </si>
+  <si>
+    <t>Flange weld collar: PN10</t>
+  </si>
+  <si>
+    <t>Flange weld collar: PN16</t>
+  </si>
+  <si>
+    <t>Flange weld collar: PN25</t>
+  </si>
+  <si>
+    <t>FLA</t>
+  </si>
+  <si>
+    <t>EN 1092-1 A1</t>
+  </si>
+  <si>
+    <t>Blind Flange: PN40</t>
+  </si>
+  <si>
+    <t>Blind Flange: PN06</t>
+  </si>
+  <si>
+    <t>Blind Flange: PN10</t>
+  </si>
+  <si>
+    <t>Blind Flange: PN16</t>
+  </si>
+  <si>
+    <t>Blind Flange: PN25</t>
+  </si>
+  <si>
+    <t>FLABL</t>
+  </si>
+  <si>
+    <t>EN 10253-2 - Elbow: 3D</t>
+  </si>
+  <si>
+    <t>EN 10253-2 - Elbow: 2D</t>
+  </si>
+  <si>
+    <t>EN 10253-2 - Elbow: 5D</t>
+  </si>
+  <si>
+    <t>BOG</t>
   </si>
 </sst>
 </file>
@@ -1800,17 +1860,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" style="1" customWidth="1"/>
     <col min="2" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1842,6 +1902,171 @@
         <v>94</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Export undefined elements release candidate
</commit_message>
<xml_diff>
--- a/revit-ntr-exporter/NTR_CONFIG.xlsx
+++ b/revit-ntr-exporter/NTR_CONFIG.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="117">
   <si>
     <t>TMONT</t>
   </si>
@@ -345,9 +345,6 @@
     <t>FLA</t>
   </si>
   <si>
-    <t>EN 1092-1 A1</t>
-  </si>
-  <si>
     <t>Blind Flange: PN40</t>
   </si>
   <si>
@@ -376,6 +373,15 @@
   </si>
   <si>
     <t>BOG</t>
+  </si>
+  <si>
+    <t>'EN 10253-2 - Type B'</t>
+  </si>
+  <si>
+    <t>'EN 10253-2'</t>
+  </si>
+  <si>
+    <t>'EN 1092-1/11/PN40'</t>
   </si>
 </sst>
 </file>
@@ -1862,15 +1868,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" style="1" customWidth="1"/>
     <col min="2" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1898,8 +1904,8 @@
       <c r="C2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>94</v>
+      <c r="D2" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1909,8 +1915,8 @@
       <c r="B3" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>94</v>
+      <c r="D3" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1920,8 +1926,8 @@
       <c r="B4" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>94</v>
+      <c r="D4" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1931,8 +1937,8 @@
       <c r="B5" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>104</v>
+      <c r="D5" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1942,8 +1948,8 @@
       <c r="B6" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>104</v>
+      <c r="D6" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1953,8 +1959,8 @@
       <c r="B7" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>104</v>
+      <c r="D7" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1964,8 +1970,8 @@
       <c r="B8" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>104</v>
+      <c r="D8" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1975,71 +1981,71 @@
       <c r="B9" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>104</v>
+      <c r="D9" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>104</v>
+      <c r="D13" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>94</v>
@@ -2047,10 +2053,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>94</v>
@@ -2058,10 +2064,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
Valve and supports release candidate
</commit_message>
<xml_diff>
--- a/revit-ntr-exporter/NTR_CONFIG.xlsx
+++ b/revit-ntr-exporter/NTR_CONFIG.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="GEN" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="IS" sheetId="10" r:id="rId6"/>
     <sheet name="PIPELINES" sheetId="11" r:id="rId7"/>
     <sheet name="ELEMENTS" sheetId="12" r:id="rId8"/>
+    <sheet name="SUPPORTS" sheetId="13" r:id="rId9"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="156">
   <si>
     <t>TMONT</t>
   </si>
@@ -315,9 +316,6 @@
     <t>H</t>
   </si>
   <si>
-    <t>EN 10253-2</t>
-  </si>
-  <si>
     <t>EN 10253-2 - Reducer: Conc.</t>
   </si>
   <si>
@@ -382,6 +380,126 @@
   </si>
   <si>
     <t>'EN 1092-1/11/PN40'</t>
+  </si>
+  <si>
+    <t>Compac: DN 150</t>
+  </si>
+  <si>
+    <t>BROEN BALLOMAX: 150 FG Håndhjul</t>
+  </si>
+  <si>
+    <t>Generic filter: DN300 PN16</t>
+  </si>
+  <si>
+    <t>Generisk-ventil: FLOWMÅLER-DN150-PN25-FL</t>
+  </si>
+  <si>
+    <t>BROEN TRUNNION: 300 Akt</t>
+  </si>
+  <si>
+    <t>Generisk-ventil: FLOWMÅLER-DN200-PN25-FL</t>
+  </si>
+  <si>
+    <t>JiP SS-SF-FF RG: DN100 SF PN25</t>
+  </si>
+  <si>
+    <t>JiP SS-SF-FF RG: DN100 FF PN25</t>
+  </si>
+  <si>
+    <t>Support Symbolic: STOP</t>
+  </si>
+  <si>
+    <t>Support Symbolic: GUI + B+</t>
+  </si>
+  <si>
+    <t>Support Symbolic: ANC</t>
+  </si>
+  <si>
+    <t>Support Symbolic: GUI + B</t>
+  </si>
+  <si>
+    <t>Support Symbolic: B+</t>
+  </si>
+  <si>
+    <t>Support Symbolic: HGR</t>
+  </si>
+  <si>
+    <t>BROEN BALLOMAX: 200 FG Akt</t>
+  </si>
+  <si>
+    <t>BROEN BALLOMAX: 150 FG Akt</t>
+  </si>
+  <si>
+    <t>Generic filter: DN200 PN25</t>
+  </si>
+  <si>
+    <t>RAA200AS: RAA200AS</t>
+  </si>
+  <si>
+    <t>ARM</t>
+  </si>
+  <si>
+    <t>GEW</t>
+  </si>
+  <si>
+    <t>31.4</t>
+  </si>
+  <si>
+    <t>224</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>431</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>65.6</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>FH</t>
+  </si>
+  <si>
+    <t>0.82</t>
+  </si>
+  <si>
+    <t>Support Symbolic: GL</t>
+  </si>
+  <si>
+    <t>GL</t>
+  </si>
+  <si>
+    <t>MALL</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>AX</t>
+  </si>
+  <si>
+    <t>FL</t>
   </si>
 </sst>
 </file>
@@ -1866,20 +1984,423 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="68.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>118</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <picture r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="68.42578125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>88</v>
@@ -1888,190 +2409,133 @@
         <v>90</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>89</v>
+        <v>151</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>91</v>
+      <c r="A2" t="s">
+        <v>124</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>114</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>95</v>
+      <c r="A3" t="s">
+        <v>125</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>115</v>
+        <v>155</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>97</v>
+      <c r="A4" t="s">
+        <v>126</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>115</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>99</v>
+      <c r="A5" t="s">
+        <v>127</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>116</v>
+        <v>155</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>100</v>
+      <c r="A6" t="s">
+        <v>128</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>116</v>
+        <v>145</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>101</v>
+      <c r="A7" t="s">
+        <v>129</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>116</v>
+        <v>147</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>102</v>
+      <c r="A8" t="s">
+        <v>149</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>116</v>
+        <v>150</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>116</v>
-      </c>
+      <c r="A9"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>116</v>
-      </c>
+      <c r="A10"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>116</v>
-      </c>
+      <c r="A11"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>116</v>
-      </c>
+      <c r="A12"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>116</v>
-      </c>
+      <c r="A13"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>116</v>
-      </c>
+      <c r="A14"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="A15"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="A16"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Must figure == out
</commit_message>
<xml_diff>
--- a/revit-ntr-exporter/NTR_CONFIG.xlsx
+++ b/revit-ntr-exporter/NTR_CONFIG.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="GEN" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="162">
   <si>
     <t>TMONT</t>
   </si>
@@ -512,6 +512,12 @@
   </si>
   <si>
     <t>Generic filter: DN350 PN16</t>
+  </si>
+  <si>
+    <t>'EN 10253-2 - Type A, concentric'</t>
+  </si>
+  <si>
+    <t>'EN 10253-2 - Type A, eccentric'</t>
   </si>
 </sst>
 </file>
@@ -1998,15 +2004,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="68.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="21.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -2049,7 +2055,7 @@
         <v>95</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>114</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2060,7 +2066,7 @@
         <v>95</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2430,7 +2436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>